<commit_message>
make bcitwo a temperate plot
</commit_message>
<xml_diff>
--- a/data_prep/input/global_metainfo/plot_sites_information.xlsx
+++ b/data_prep/input/global_metainfo/plot_sites_information.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisahulsmann/Dropbox/Work/Publications ongoing/2022 Huelsmann CNDD dynamic/analysis/data_prep/ForestGEO_datacleaning@git/global_metainfo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisahulsmann/Dropbox/Work/Publications ongoing/2022 Huelsmann CNDD dynamic/analysis/latitudinalCNDD@git/data_prep/input/global_metainfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6A88C5-217C-7143-AD68-2934F17DCA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0944BBAE-8E1B-9441-941B-6A2F8B56BE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19460" xr2:uid="{30C046F3-23A7-D84A-9C76-120555F59374}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>site</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Barro Colorado Island 1</t>
+  </si>
+  <si>
+    <t>temperate</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="37" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -773,13 +776,13 @@
         <v>500</v>
       </c>
       <c r="L3" s="2">
-        <v>9.1542999999999992</v>
+        <v>45</v>
       </c>
       <c r="M3" s="2">
         <v>-79.846100000000007</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="O3" s="2">
         <v>120</v>

</xml_diff>